<commit_message>
updated calculations from datasheet
</commit_message>
<xml_diff>
--- a/doc/LM5060_calculation.xlsx
+++ b/doc/LM5060_calculation.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="23440" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Datasheet" sheetId="2" r:id="rId1"/>
+    <sheet name="Archive_wrong" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>UVLO</t>
   </si>
@@ -72,6 +73,75 @@
   </si>
   <si>
     <t>Component Selection</t>
+  </si>
+  <si>
+    <t>UVLO-IBIAS (µA)</t>
+  </si>
+  <si>
+    <t>UVLO-TH(V)</t>
+  </si>
+  <si>
+    <t>VINMIN(V)</t>
+  </si>
+  <si>
+    <t>OVP-TH(V)</t>
+  </si>
+  <si>
+    <t>VINMAX(V)</t>
+  </si>
+  <si>
+    <t>R1(kΩ)</t>
+  </si>
+  <si>
+    <t>R2(kΩ)</t>
+  </si>
+  <si>
+    <t>R3(kΩ)</t>
+  </si>
+  <si>
+    <t>Numerator</t>
+  </si>
+  <si>
+    <t>Denominator</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Pick &amp; Evaluate</t>
+  </si>
+  <si>
+    <t>OVPHYS-TH(V)</t>
+  </si>
+  <si>
+    <t>VINMAX-TURNOFF(V)</t>
+  </si>
+  <si>
+    <t>VINMAX-RECOVER(V)</t>
+  </si>
+  <si>
+    <t>Solve &amp; Design</t>
+  </si>
+  <si>
+    <t>Procedure to design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Use the Solve &amp; Design secion to </t>
+  </si>
+  <si>
+    <t>evaluate R1,R2,R3 based on VIN spec</t>
+  </si>
+  <si>
+    <t>2- Use the Pick &amp; Evaluate section to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dial in actual resistor values and </t>
+  </si>
+  <si>
+    <t>evaluate VIN specs</t>
+  </si>
+  <si>
+    <t>Datasheet Parameters</t>
   </si>
 </sst>
 </file>
@@ -79,7 +149,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -114,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,8 +209,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -148,24 +230,165 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -179,6 +402,87 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7874000" y="152400"/>
+          <a:ext cx="4699000" cy="3797300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10223500" y="4038600"/>
+          <a:ext cx="13169900" cy="7645400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -484,10 +788,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="31" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="19">
+        <v>5.5</v>
+      </c>
+      <c r="D3">
+        <f>0.000001*C3</f>
+        <v>5.4999999999999999E-6</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="19">
+        <v>1.6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="19">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="20">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="14">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="14">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="14">
+        <v>69</v>
+      </c>
+      <c r="D11">
+        <f>1000*C11</f>
+        <v>69000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="16">
+        <f>D12/1000</f>
+        <v>10.625056420409331</v>
+      </c>
+      <c r="D12">
+        <f>E12/F12</f>
+        <v>10625.056420409332</v>
+      </c>
+      <c r="E12">
+        <f>(D13*C10)/C5-D13-D11-(D3*D11*D13)/C5</f>
+        <v>10625.056420409332</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="18">
+        <f>D13/1000</f>
+        <v>6.0504212625451146</v>
+      </c>
+      <c r="D13">
+        <f>E13/F13</f>
+        <v>6050.4212625451146</v>
+      </c>
+      <c r="E13">
+        <f>D11+(C4*D11)/(C9-C4-D3*D11)</f>
+        <v>85675.477682954457</v>
+      </c>
+      <c r="F13">
+        <f>(C10/C5)-(D3*D11/C5)</f>
+        <v>14.16025</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="H16" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="14">
+        <v>66.5</v>
+      </c>
+      <c r="D17">
+        <f>1000*C17</f>
+        <v>66500</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="14">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:D19" si="0">1000*C18</f>
+        <v>14000</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="14">
+        <v>6.04</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>6040</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="13"/>
+      <c r="C20" s="15"/>
+      <c r="H20" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="16">
+        <f>C4+D17*(D3+C4/(D18+D19))</f>
+        <v>7.2751312375249508</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="13"/>
+      <c r="C22" s="15"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="16">
+        <f>D17*(D3+C5/D19)+D18*C5/D19+C5</f>
+        <v>29.021379139072849</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="18">
+        <f>D17*(D3+C6/D19)+D18*C6/D19+C6</f>
+        <v>25.582703642384111</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated and verified LM5060 calculations vs measurements
</commit_message>
<xml_diff>
--- a/doc/LM5060_calculation.xlsx
+++ b/doc/LM5060_calculation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="23440" tabRatio="500"/>
+    <workbookView xWindow="2400" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Datasheet" sheetId="2" r:id="rId1"/>
@@ -359,12 +359,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -373,6 +367,12 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -790,7 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
@@ -806,16 +806,16 @@
   <sheetData>
     <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="17">
         <v>5.5</v>
       </c>
       <c r="D3">
@@ -827,10 +827,10 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="17">
         <v>1.6</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -838,10 +838,10 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="17">
         <v>2</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -849,19 +849,19 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="18">
         <v>1.76</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="20"/>
       <c r="D8" t="s">
         <v>25</v>
       </c>
@@ -873,26 +873,26 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="12">
         <v>8.6</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="12">
         <v>28.7</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="12">
         <v>69</v>
       </c>
       <c r="D11">
@@ -901,10 +901,10 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="14">
         <f>D12/1000</f>
         <v>10.625056420409331</v>
       </c>
@@ -921,10 +921,10 @@
       </c>
     </row>
     <row r="13" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="16">
         <f>D13/1000</f>
         <v>6.0504212625451146</v>
       </c>
@@ -943,19 +943,19 @@
     </row>
     <row r="15" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="20"/>
       <c r="H16" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="12">
         <v>66.5</v>
       </c>
       <c r="D17">
@@ -967,10 +967,10 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="12">
         <v>14</v>
       </c>
       <c r="D18">
@@ -982,10 +982,10 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="12">
         <v>6.04</v>
       </c>
       <c r="D19">
@@ -997,17 +997,17 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="13"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="13"/>
       <c r="H20" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="14">
         <f>C4+D17*(D3+C4/(D18+D19))</f>
         <v>7.2751312375249508</v>
       </c>
@@ -1016,23 +1016,23 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="13"/>
-      <c r="C22" s="15"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="14">
         <f>D17*(D3+C5/D19)+D18*C5/D19+C5</f>
         <v>29.021379139072849</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="16">
         <f>D17*(D3+C6/D19)+D18*C6/D19+C6</f>
         <v>25.582703642384111</v>
       </c>

</xml_diff>

<commit_message>
updated LM5060 calculations and restored pin map
</commit_message>
<xml_diff>
--- a/doc/LM5060_calculation.xlsx
+++ b/doc/LM5060_calculation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Datasheet" sheetId="2" r:id="rId1"/>
@@ -791,7 +791,7 @@
   <dimension ref="B1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -877,7 +877,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="12">
-        <v>8.6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
@@ -885,7 +885,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="12">
-        <v>28.7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
@@ -893,11 +893,11 @@
         <v>20</v>
       </c>
       <c r="C11" s="12">
-        <v>69</v>
+        <v>66.5</v>
       </c>
       <c r="D11">
         <f>1000*C11</f>
-        <v>69000</v>
+        <v>66500</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
@@ -906,15 +906,15 @@
       </c>
       <c r="C12" s="14">
         <f>D12/1000</f>
-        <v>10.625056420409331</v>
+        <v>11.068596509390572</v>
       </c>
       <c r="D12">
         <f>E12/F12</f>
-        <v>10625.056420409332</v>
+        <v>11068.596509390572</v>
       </c>
       <c r="E12">
         <f>(D13*C10)/C5-D13-D11-(D3*D11*D13)/C5</f>
-        <v>10625.056420409332</v>
+        <v>11068.596509390572</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -926,19 +926,19 @@
       </c>
       <c r="C13" s="16">
         <f>D13/1000</f>
-        <v>6.0504212625451146</v>
+        <v>6.5640836082710967</v>
       </c>
       <c r="D13">
         <f>E13/F13</f>
-        <v>6050.4212625451146</v>
+        <v>6564.0836082710966</v>
       </c>
       <c r="E13">
         <f>D11+(C4*D11)/(C9-C4-D3*D11)</f>
-        <v>85675.477682954457</v>
+        <v>84132.680117661686</v>
       </c>
       <c r="F13">
         <f>(C10/C5)-(D3*D11/C5)</f>
-        <v>14.16025</v>
+        <v>12.817125000000001</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -971,11 +971,11 @@
         <v>21</v>
       </c>
       <c r="C18" s="12">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D18">
         <f t="shared" ref="D18:D19" si="0">1000*C18</f>
-        <v>14000</v>
+        <v>11000</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>33</v>
@@ -986,11 +986,11 @@
         <v>22</v>
       </c>
       <c r="C19" s="12">
-        <v>6.04</v>
+        <v>6.49</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>6040</v>
+        <v>6490</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>34</v>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="C21" s="14">
         <f>C4+D17*(D3+C4/(D18+D19))</f>
-        <v>7.2751312375249508</v>
+        <v>8.0492262721555168</v>
       </c>
       <c r="H21" s="10" t="s">
         <v>36</v>
@@ -1025,7 +1025,7 @@
       </c>
       <c r="C23" s="14">
         <f>D17*(D3+C5/D19)+D18*C5/D19+C5</f>
-        <v>29.021379139072849</v>
+        <v>26.248646764252697</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="C24" s="16">
         <f>D17*(D3+C6/D19)+D18*C6/D19+C6</f>
-        <v>25.582703642384111</v>
+        <v>23.142699152542374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>